<commit_message>
Aggiornato reworkpd.xlsx da lbianco via Streamlit
</commit_message>
<xml_diff>
--- a/reworkpd.xlsx
+++ b/reworkpd.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="205">
   <si>
     <t>Codice</t>
   </si>
@@ -628,6 +628,9 @@
   </si>
   <si>
     <t>TUSA MAURIZIO</t>
+  </si>
+  <si>
+    <t>Bianco Luca</t>
   </si>
 </sst>
 </file>
@@ -663,8 +666,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -959,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CP6"/>
+  <dimension ref="A1:CP7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2671,6 +2675,290 @@
         <v>104</v>
       </c>
       <c r="CP6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:94">
+      <c r="A7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7">
+        <v>92225649</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J7" t="s">
+        <v>103</v>
+      </c>
+      <c r="K7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L7" t="s">
+        <v>105</v>
+      </c>
+      <c r="M7" t="s">
+        <v>106</v>
+      </c>
+      <c r="N7" t="s">
+        <v>104</v>
+      </c>
+      <c r="O7" s="1">
+        <v>45889</v>
+      </c>
+      <c r="P7" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>191</v>
+      </c>
+      <c r="R7" t="s">
+        <v>110</v>
+      </c>
+      <c r="S7" t="s">
+        <v>111</v>
+      </c>
+      <c r="T7" t="s">
+        <v>204</v>
+      </c>
+      <c r="U7" t="s">
+        <v>192</v>
+      </c>
+      <c r="V7" t="s">
+        <v>104</v>
+      </c>
+      <c r="W7" t="s">
+        <v>114</v>
+      </c>
+      <c r="X7" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>193</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>194</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>195</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>196</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>122</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>171</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>197</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>173</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>198</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>127</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BC7" t="s">
+        <v>128</v>
+      </c>
+      <c r="BD7" t="s">
+        <v>129</v>
+      </c>
+      <c r="BE7" t="s">
+        <v>199</v>
+      </c>
+      <c r="BF7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BG7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BH7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BI7" t="s">
+        <v>200</v>
+      </c>
+      <c r="BJ7" t="s">
+        <v>110</v>
+      </c>
+      <c r="BK7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BL7" t="s">
+        <v>131</v>
+      </c>
+      <c r="BM7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BN7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BO7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BP7" t="s">
+        <v>99</v>
+      </c>
+      <c r="BQ7" t="s">
+        <v>132</v>
+      </c>
+      <c r="BR7" t="s">
+        <v>99</v>
+      </c>
+      <c r="BS7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BT7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BU7" t="s">
+        <v>133</v>
+      </c>
+      <c r="BV7" t="s">
+        <v>114</v>
+      </c>
+      <c r="BW7" t="s">
+        <v>114</v>
+      </c>
+      <c r="BX7" t="s">
+        <v>104</v>
+      </c>
+      <c r="BY7" t="s">
+        <v>134</v>
+      </c>
+      <c r="BZ7" t="s">
+        <v>104</v>
+      </c>
+      <c r="CA7" t="s">
+        <v>104</v>
+      </c>
+      <c r="CB7" t="s">
+        <v>104</v>
+      </c>
+      <c r="CC7" t="s">
+        <v>201</v>
+      </c>
+      <c r="CD7" t="s">
+        <v>99</v>
+      </c>
+      <c r="CE7" t="s">
+        <v>114</v>
+      </c>
+      <c r="CF7" t="s">
+        <v>104</v>
+      </c>
+      <c r="CG7" t="s">
+        <v>104</v>
+      </c>
+      <c r="CH7" t="s">
+        <v>104</v>
+      </c>
+      <c r="CI7" t="s">
+        <v>102</v>
+      </c>
+      <c r="CJ7" t="s">
+        <v>104</v>
+      </c>
+      <c r="CK7" t="s">
+        <v>104</v>
+      </c>
+      <c r="CL7" t="s">
+        <v>104</v>
+      </c>
+      <c r="CM7" t="s">
+        <v>202</v>
+      </c>
+      <c r="CN7" t="s">
+        <v>104</v>
+      </c>
+      <c r="CO7" t="s">
+        <v>104</v>
+      </c>
+      <c r="CP7" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>